<commit_message>
[update] regenerate att tables
</commit_message>
<xml_diff>
--- a/Yujie-plot/其他/datasetAttTable/UAV20L_att.xlsx
+++ b/Yujie-plot/其他/datasetAttTable/UAV20L_att.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\hyj-small-repo\v4r-matlab-plot\其他\datasetAttTable\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\hyj-small-repo\v4r-matlab-plot\Yujie-plot\其他\datasetAttTable\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{43C1637B-DBF0-4155-806E-4642E80D8DAE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C50A8068-F2C5-4E6C-8370-1EFF7ED572C1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="732" yWindow="732" windowWidth="16404" windowHeight="9420" xr2:uid="{7BDA0C15-32A3-455C-9F3B-A827CF9D482D}"/>
+    <workbookView xWindow="1428" yWindow="1428" windowWidth="16404" windowHeight="9420" xr2:uid="{035F8D55-7425-4245-910A-6E611CD97D16}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -101,40 +101,40 @@
     <t>frameNum</t>
   </si>
   <si>
+    <t>SV</t>
+  </si>
+  <si>
     <t>ARC</t>
   </si>
   <si>
+    <t>LR</t>
+  </si>
+  <si>
+    <t>FM</t>
+  </si>
+  <si>
+    <t>FOC</t>
+  </si>
+  <si>
+    <t>POC</t>
+  </si>
+  <si>
+    <t>OV</t>
+  </si>
+  <si>
     <t>BC</t>
   </si>
   <si>
+    <t>IV</t>
+  </si>
+  <si>
+    <t>VC</t>
+  </si>
+  <si>
     <t>CM</t>
   </si>
   <si>
-    <t>FM</t>
-  </si>
-  <si>
-    <t>FOC</t>
-  </si>
-  <si>
-    <t>IV</t>
-  </si>
-  <si>
-    <t>LR</t>
-  </si>
-  <si>
-    <t>OV</t>
-  </si>
-  <si>
-    <t>POC</t>
-  </si>
-  <si>
-    <t>SV</t>
-  </si>
-  <si>
     <t>SOB</t>
-  </si>
-  <si>
-    <t>VC</t>
   </si>
 </sst>
 </file>
@@ -497,7 +497,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0461977-0071-4CD2-839F-1806C4F80C2E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A124D97-C7AE-463D-BDE1-AA1EE91CF5F3}">
   <dimension ref="A1:N21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -506,18 +506,18 @@
   <cols>
     <col min="1" max="1" width="9.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="3.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="4.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="3.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="3.5546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="4.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="5.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="3.21875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="3.5546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="4.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="5.44140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="3.77734375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="5.21875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="3.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="3.21875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="4" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="4.5546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="5.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -1451,7 +1451,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF8FD99F-8A30-4821-A590-900FF3E13F8A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2AE870C-C376-45B3-A6E1-C2F83408C18A}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1464,7 +1464,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82D3003F-C82E-4A08-A30B-75CC843B10F1}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F855121A-6765-4FC4-8E8F-85B8F389183E}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>